<commit_message>
Added extra pin to J1 connector to make it surface mount, BOM Complete except for xtals.
</commit_message>
<xml_diff>
--- a/Hardware/Processor/Processor_BOM.xlsx
+++ b/Hardware/Processor/Processor_BOM.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Processor" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="147">
   <si>
     <t>Reference</t>
   </si>
@@ -168,9 +168,6 @@
     <t xml:space="preserve">R14 R17 R19 R21 R22 </t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>27R</t>
   </si>
   <si>
@@ -259,6 +256,210 @@
   </si>
   <si>
     <t>Check pinout at footprint assignment</t>
+  </si>
+  <si>
+    <t>961240-6300-AR-PR</t>
+  </si>
+  <si>
+    <t>3M9499CT-ND</t>
+  </si>
+  <si>
+    <t>Surface Mount</t>
+  </si>
+  <si>
+    <t>2x20 Male Header</t>
+  </si>
+  <si>
+    <t>2x12 Male Header</t>
+  </si>
+  <si>
+    <t>Uses leftover pins of J1</t>
+  </si>
+  <si>
+    <t>961120-6300-AR-PR</t>
+  </si>
+  <si>
+    <t>3M9492CT-ND</t>
+  </si>
+  <si>
+    <t>2x10 Male Header</t>
+  </si>
+  <si>
+    <t>1x3 Male Header</t>
+  </si>
+  <si>
+    <t>1x4 Male Header</t>
+  </si>
+  <si>
+    <t>Surface Mount, 0.05" pitch</t>
+  </si>
+  <si>
+    <t>3x Quantity</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>BSS806NEH6327XTSA1</t>
+  </si>
+  <si>
+    <t>BSS806NEH6327XTSA1CT-ND</t>
+  </si>
+  <si>
+    <t>PRTR5V0U2X,215</t>
+  </si>
+  <si>
+    <t>TO-253-4</t>
+  </si>
+  <si>
+    <t>568-4140-1-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10KGRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-071ML</t>
+  </si>
+  <si>
+    <t>311-1.0MGRCT-ND</t>
+  </si>
+  <si>
+    <t>C0603C104M5RACTU</t>
+  </si>
+  <si>
+    <t>399-7845-1-ND</t>
+  </si>
+  <si>
+    <t>3342</t>
+  </si>
+  <si>
+    <t>TL3342F160QG/TR</t>
+  </si>
+  <si>
+    <t>EG2531CT-ND</t>
+  </si>
+  <si>
+    <t>MSOP-8</t>
+  </si>
+  <si>
+    <t>TXS0102DCTT</t>
+  </si>
+  <si>
+    <t>296-32603-1-ND</t>
+  </si>
+  <si>
+    <t>TQFP-144 (20x20)</t>
+  </si>
+  <si>
+    <t>ATSAM4E16EA-AURCT-ND</t>
+  </si>
+  <si>
+    <t>ATSAM4E16EA-AUR</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>LM3671MF-3.3/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>LM3671MF-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>296-20887-1-ND</t>
+  </si>
+  <si>
+    <t>LM4040C30IDBZR</t>
+  </si>
+  <si>
+    <t>3M9497CT-ND</t>
+  </si>
+  <si>
+    <t>961224-6300-AR-PR</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>USB Micro SMT</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>1/8 Watt</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>LTST-C170KSKT</t>
+  </si>
+  <si>
+    <t>160-1416-1-ND</t>
+  </si>
+  <si>
+    <t>LQH3NPN100MJ0L</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>490-11681-1-ND</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>311-1085-1-ND</t>
+  </si>
+  <si>
+    <t>311-150ARCT-ND</t>
+  </si>
+  <si>
+    <t>311-1.0GRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-071RL</t>
+  </si>
+  <si>
+    <t>490-9749-1-ND</t>
+  </si>
+  <si>
+    <t>GRM21BR60J475KA11L</t>
+  </si>
+  <si>
+    <t>CL10B472KB8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1098-1-ND</t>
+  </si>
+  <si>
+    <t>490-1717-1-ND</t>
+  </si>
+  <si>
+    <t>GRM21BR60J106KE19L</t>
+  </si>
+  <si>
+    <t>GRM21BR60J225KA01L</t>
+  </si>
+  <si>
+    <t>490-1712-1-ND</t>
+  </si>
+  <si>
+    <t>150R</t>
+  </si>
+  <si>
+    <t>CDRH2D14NP-2R2NC</t>
+  </si>
+  <si>
+    <t>308-2294-1-ND</t>
   </si>
 </sst>
 </file>
@@ -742,7 +943,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -771,6 +972,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -816,18 +1018,12 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -838,6 +1034,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -856,16 +1062,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:H37" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:H37"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Reference" dataDxfId="2"/>
-    <tableColumn id="2" name=" Quantity" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:I37" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="B2:I37"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Reference" dataDxfId="7"/>
+    <tableColumn id="2" name=" Quantity" dataDxfId="6"/>
+    <tableColumn id="8" name="3x Quantity" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[ Quantity]]*3</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="3" name=" Value" dataDxfId="1"/>
-    <tableColumn id="4" name=" Footprint" dataDxfId="3"/>
-    <tableColumn id="5" name="MFG#" dataDxfId="7"/>
-    <tableColumn id="6" name="DigiKey#" dataDxfId="6"/>
-    <tableColumn id="7" name="Comments" dataDxfId="5"/>
+    <tableColumn id="4" name=" Footprint" dataDxfId="5"/>
+    <tableColumn id="5" name="MFG#" dataDxfId="4"/>
+    <tableColumn id="6" name="DigiKey#" dataDxfId="3"/>
+    <tableColumn id="7" name="Comments" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1168,23 +1377,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H40"/>
+  <dimension ref="B2:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="55.5703125" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1192,580 +1402,910 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>72</v>
       </c>
-      <c r="H2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="F3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="7">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>72</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>5</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="7">
         <v>2</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="7">
         <v>1</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="7">
         <v>4</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="7">
         <v>1</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="F24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>5</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
+      <c r="D26" s="8">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>9</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+      <c r="F26" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="7">
-        <v>3</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C28" s="7">
         <v>12</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>36</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="7">
         <v>2</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C30" s="7">
         <v>1</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="7">
         <v>1</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C32" s="7">
         <v>1</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C34" s="7">
         <v>1</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+      <c r="D35" s="7">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+      <c r="D36" s="8">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="7">
+      <c r="F36" s="6"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="8">
         <v>1</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+      <c r="D37" s="8">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="7">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="6"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C38" s="9"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished BOM. Generated new netlist w/ new component footprints
</commit_message>
<xml_diff>
--- a/Hardware/Processor/Processor_BOM.xlsx
+++ b/Hardware/Processor/Processor_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="170">
   <si>
     <t>Reference</t>
   </si>
@@ -36,15 +36,9 @@
     <t xml:space="preserve">C10 C11 </t>
   </si>
   <si>
-    <t>3.9pF</t>
-  </si>
-  <si>
     <t xml:space="preserve">C19 C20 </t>
   </si>
   <si>
-    <t>18pF</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1 C12 C14 C15 C16 C18 C21 C23 C24 C26 C27 C29 C3 C30 C32 C33 C36 C37 C38 C39 C5 C6 C8 C9 </t>
   </si>
   <si>
@@ -460,6 +454,81 @@
   </si>
   <si>
     <t>308-2294-1-ND</t>
+  </si>
+  <si>
+    <t>20021121-00010T4LF</t>
+  </si>
+  <si>
+    <t>609-3729-ND</t>
+  </si>
+  <si>
+    <t>Ccrystal (12 MHz) must be 12.5 to 17.5 pF</t>
+  </si>
+  <si>
+    <t>Ccrystal (RTC) must be 6 to 12.5 pF</t>
+  </si>
+  <si>
+    <t>Cext = 2 × (Ccrystal - Cpara - Cpcb)</t>
+  </si>
+  <si>
+    <t>Cpara (RTC) = 0.7pF</t>
+  </si>
+  <si>
+    <t>Cpcb (6 mil trace, 2 layer board above gnd plane, 1.6 mm, 4mm trace) = 0.5 pF. Keep traces &lt; 5mm and we will be ok</t>
+  </si>
+  <si>
+    <t>Cpara (12 MHz) = &lt;0.1pF</t>
+  </si>
+  <si>
+    <t>HC49</t>
+  </si>
+  <si>
+    <t>GC1200050</t>
+  </si>
+  <si>
+    <t>GC1200050CT-ND</t>
+  </si>
+  <si>
+    <t>Cext (12 MHz) = 2 * (16 pF - 9.5 - 0.5 pF) = 12 pF</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>SER4103CT-ND</t>
+  </si>
+  <si>
+    <t>FC-135 32.7680KA-A5</t>
+  </si>
+  <si>
+    <t>12.5 pF</t>
+  </si>
+  <si>
+    <t>16 pF</t>
+  </si>
+  <si>
+    <t>Cext (RTC) = 2 * (12.5 pF - 0.7 pF - 0.5 pF) = 22.6</t>
+  </si>
+  <si>
+    <t>27 pF</t>
+  </si>
+  <si>
+    <t>C0603C270F5GACTU</t>
+  </si>
+  <si>
+    <t>399-7888-1-ND</t>
+  </si>
+  <si>
+    <t>1276-2175-1-ND</t>
+  </si>
+  <si>
+    <t>CL10C120FB8NNNC</t>
+  </si>
+  <si>
+    <t>311-27.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-0727RL</t>
   </si>
 </sst>
 </file>
@@ -943,7 +1012,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -951,28 +1020,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1020,13 +1079,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1038,6 +1090,13 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1067,14 +1126,14 @@
   <tableColumns count="8">
     <tableColumn id="1" name="Reference" dataDxfId="7"/>
     <tableColumn id="2" name=" Quantity" dataDxfId="6"/>
-    <tableColumn id="8" name="3x Quantity" dataDxfId="0">
+    <tableColumn id="8" name="3x Quantity" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[ Quantity]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name=" Value" dataDxfId="1"/>
-    <tableColumn id="4" name=" Footprint" dataDxfId="5"/>
-    <tableColumn id="5" name="MFG#" dataDxfId="4"/>
-    <tableColumn id="6" name="DigiKey#" dataDxfId="3"/>
-    <tableColumn id="7" name="Comments" dataDxfId="2"/>
+    <tableColumn id="3" name=" Value" dataDxfId="4"/>
+    <tableColumn id="4" name=" Footprint" dataDxfId="3"/>
+    <tableColumn id="5" name="MFG#" dataDxfId="2"/>
+    <tableColumn id="6" name="DigiKey#" dataDxfId="1"/>
+    <tableColumn id="7" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1377,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I40"/>
+  <dimension ref="B2:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="B3" sqref="B3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1411,901 +1470,943 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="G3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>6</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="5" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="7">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4">
         <v>24</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>124</v>
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>74</v>
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="7">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
         <v>2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>124</v>
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="7">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>124</v>
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4">
         <v>7</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>74</v>
+        <v>17</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7">
-        <v>5</v>
-      </c>
-      <c r="D11" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" t="s">
         <v>126</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
         <v>127</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>6</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="G22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D24">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="7">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="7">
-        <v>4</v>
-      </c>
-      <c r="D23" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="7">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="2"/>
+      <c r="F24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" t="s">
+        <v>98</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" t="s">
+        <v>169</v>
+      </c>
+      <c r="H26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="7">
-        <v>5</v>
-      </c>
-      <c r="D25" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" t="s">
         <v>133</v>
       </c>
-      <c r="H25" t="s">
-        <v>133</v>
-      </c>
-      <c r="I25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="H27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" t="s">
+        <v>111</v>
+      </c>
+      <c r="G34" t="s">
+        <v>113</v>
+      </c>
+      <c r="H34" t="s">
+        <v>112</v>
+      </c>
+      <c r="I34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
-      <c r="D26" s="8">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>9</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="7">
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36">
         <v>1</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D36">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="7">
-        <v>12</v>
-      </c>
-      <c r="D28" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>36</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="7">
-        <v>2</v>
-      </c>
-      <c r="D29" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>6</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="7">
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" t="s">
+        <v>159</v>
+      </c>
+      <c r="H36" t="s">
+        <v>158</v>
+      </c>
+      <c r="I36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D37">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1</v>
-      </c>
-      <c r="D32" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="7">
-        <v>1</v>
-      </c>
-      <c r="D33" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="7">
-        <v>1</v>
-      </c>
-      <c r="D34" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="7">
-        <v>1</v>
-      </c>
-      <c r="D35" s="7">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="8">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="E37" t="s">
         <v>67</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="8">
-        <v>1</v>
-      </c>
-      <c r="D37" s="8">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>3</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
+        <v>154</v>
+      </c>
+      <c r="H37" t="s">
+        <v>155</v>
+      </c>
+      <c r="I37" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
+      <c r="B40" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated BOM & Netlist. Started PCB Layout
</commit_message>
<xml_diff>
--- a/Hardware/Processor/Processor_BOM.xlsx
+++ b/Hardware/Processor/Processor_BOM.xlsx
@@ -1079,6 +1079,16 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1093,16 +1103,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1124,16 +1124,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:I37" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="B2:I37"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Reference" dataDxfId="7"/>
-    <tableColumn id="2" name=" Quantity" dataDxfId="6"/>
-    <tableColumn id="8" name="3x Quantity" dataDxfId="5">
+    <tableColumn id="1" name="Reference" dataDxfId="2"/>
+    <tableColumn id="2" name=" Quantity" dataDxfId="0"/>
+    <tableColumn id="8" name="3x Quantity" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[ Quantity]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name=" Value" dataDxfId="4"/>
-    <tableColumn id="4" name=" Footprint" dataDxfId="3"/>
-    <tableColumn id="5" name="MFG#" dataDxfId="2"/>
-    <tableColumn id="6" name="DigiKey#" dataDxfId="1"/>
-    <tableColumn id="7" name="Comments" dataDxfId="0"/>
+    <tableColumn id="3" name=" Value" dataDxfId="7"/>
+    <tableColumn id="4" name=" Footprint" dataDxfId="6"/>
+    <tableColumn id="5" name="MFG#" dataDxfId="5"/>
+    <tableColumn id="6" name="DigiKey#" dataDxfId="4"/>
+    <tableColumn id="7" name="Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1439,7 +1439,7 @@
   <dimension ref="B2:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I4"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,7 +1483,7 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
       <c r="D3">
@@ -1507,7 +1507,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
       <c r="D4">
@@ -1708,10 +1708,10 @@
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>6</v>
       </c>
@@ -1735,10 +1735,10 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1762,10 +1762,10 @@
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1786,10 +1786,10 @@
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1813,10 +1813,10 @@
       <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>1</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1840,10 +1840,10 @@
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1867,10 +1867,10 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1891,10 +1891,10 @@
       <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1918,10 +1918,10 @@
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1945,10 +1945,10 @@
       <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1969,10 +1969,10 @@
       <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -1993,10 +1993,10 @@
       <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>4</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>12</v>
       </c>
@@ -2020,10 +2020,10 @@
       <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>1</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2044,10 +2044,10 @@
       <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>5</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>15</v>
       </c>
@@ -2071,10 +2071,10 @@
       <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>3</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>9</v>
       </c>
@@ -2095,10 +2095,10 @@
       <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2119,10 +2119,10 @@
       <c r="B28" t="s">
         <v>50</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>12</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>36</v>
       </c>
@@ -2143,10 +2143,10 @@
       <c r="B29" t="s">
         <v>74</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>2</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>6</v>
       </c>
@@ -2167,10 +2167,10 @@
       <c r="B30" t="s">
         <v>53</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="4">
         <v>1</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2191,10 +2191,10 @@
       <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2215,10 +2215,10 @@
       <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="4">
         <v>1</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2239,10 +2239,10 @@
       <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="4">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2266,10 +2266,10 @@
       <c r="B34" t="s">
         <v>62</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="4">
         <v>1</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2293,10 +2293,10 @@
       <c r="B35" t="s">
         <v>73</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="4">
         <v>1</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2317,10 +2317,10 @@
       <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="4">
         <v>1</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>
@@ -2344,10 +2344,10 @@
       <c r="B37" t="s">
         <v>66</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="4">
         <v>1</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <f>Table1[[#This Row],[ Quantity]]*3</f>
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Completed initial component placement
</commit_message>
<xml_diff>
--- a/Hardware/Processor/Processor_BOM.xlsx
+++ b/Hardware/Processor/Processor_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="171">
   <si>
     <t>Reference</t>
   </si>
@@ -39,9 +39,6 @@
     <t xml:space="preserve">C19 C20 </t>
   </si>
   <si>
-    <t xml:space="preserve">C1 C12 C14 C15 C16 C18 C21 C23 C24 C26 C27 C29 C3 C30 C32 C33 C36 C37 C38 C39 C5 C6 C8 C9 </t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -529,6 +526,12 @@
   </si>
   <si>
     <t>RC0603FR-0727RL</t>
+  </si>
+  <si>
+    <t>C29 no longer exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1 C12 C14 C15 C16 C18 C21 C23 C24 C26 C27 C3 C30 C32 C33 C36 C37 C38 C39 C5 C6 C8 C9 </t>
   </si>
 </sst>
 </file>
@@ -1079,16 +1082,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1103,6 +1096,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1124,16 +1127,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:I37" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="B2:I37"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Reference" dataDxfId="2"/>
-    <tableColumn id="2" name=" Quantity" dataDxfId="0"/>
-    <tableColumn id="8" name="3x Quantity" dataDxfId="1">
+    <tableColumn id="1" name="Reference" dataDxfId="7"/>
+    <tableColumn id="2" name=" Quantity" dataDxfId="6"/>
+    <tableColumn id="8" name="3x Quantity" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[ Quantity]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name=" Value" dataDxfId="7"/>
-    <tableColumn id="4" name=" Footprint" dataDxfId="6"/>
-    <tableColumn id="5" name="MFG#" dataDxfId="5"/>
-    <tableColumn id="6" name="DigiKey#" dataDxfId="4"/>
-    <tableColumn id="7" name="Comments" dataDxfId="3"/>
+    <tableColumn id="3" name=" Value" dataDxfId="4"/>
+    <tableColumn id="4" name=" Footprint" dataDxfId="3"/>
+    <tableColumn id="5" name="MFG#" dataDxfId="2"/>
+    <tableColumn id="6" name="DigiKey#" dataDxfId="1"/>
+    <tableColumn id="7" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1439,7 +1442,7 @@
   <dimension ref="B2:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1470,13 +1473,13 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
         <v>68</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>69</v>
-      </c>
-      <c r="I2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1491,16 +1494,16 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
         <v>163</v>
       </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>164</v>
-      </c>
-      <c r="H3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1515,46 +1518,48 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="4">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4">
+        <f>Table1[[#This Row],[ Quantity]]*3</f>
+        <v>69</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4">
-        <f>Table1[[#This Row],[ Quantity]]*3</f>
-        <v>72</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1564,22 +1569,22 @@
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1589,22 +1594,22 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
@@ -1614,22 +1619,22 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -1639,22 +1644,22 @@
         <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4">
         <v>7</v>
@@ -1664,22 +1669,22 @@
         <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4">
         <v>5</v>
@@ -1689,24 +1694,24 @@
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
@@ -1716,24 +1721,24 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
         <v>83</v>
       </c>
-      <c r="H12" t="s">
-        <v>84</v>
-      </c>
       <c r="I12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -1743,24 +1748,24 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -1770,21 +1775,21 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" t="s">
         <v>119</v>
-      </c>
-      <c r="G14" t="s">
-        <v>118</v>
-      </c>
-      <c r="H14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -1794,24 +1799,24 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" t="s">
         <v>145</v>
       </c>
-      <c r="H15" t="s">
-        <v>146</v>
-      </c>
       <c r="I15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
@@ -1821,24 +1826,24 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" t="s">
         <v>77</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>78</v>
-      </c>
-      <c r="I16" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -1848,24 +1853,24 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -1875,21 +1880,21 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
         <v>78</v>
-      </c>
-      <c r="I18" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
@@ -1899,24 +1904,24 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" t="s">
         <v>77</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>78</v>
-      </c>
-      <c r="I19" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
@@ -1926,24 +1931,24 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -1953,21 +1958,21 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" t="s">
         <v>127</v>
-      </c>
-      <c r="G21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H21" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -1977,21 +1982,21 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" t="s">
         <v>143</v>
-      </c>
-      <c r="H22" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="4">
         <v>4</v>
@@ -2001,24 +2006,24 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" t="s">
         <v>75</v>
-      </c>
-      <c r="G23" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -2028,21 +2033,21 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" t="s">
         <v>98</v>
-      </c>
-      <c r="H24" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="4">
         <v>5</v>
@@ -2052,24 +2057,24 @@
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="4">
         <v>3</v>
@@ -2079,21 +2084,21 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -2103,21 +2108,21 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="4">
         <v>12</v>
@@ -2127,21 +2132,21 @@
         <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" t="s">
         <v>96</v>
-      </c>
-      <c r="H28" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="4">
         <v>2</v>
@@ -2151,21 +2156,21 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" t="s">
         <v>102</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>103</v>
-      </c>
-      <c r="H29" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
@@ -2175,21 +2180,21 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" t="s">
         <v>102</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>103</v>
-      </c>
-      <c r="H30" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
@@ -2199,21 +2204,21 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" t="s">
         <v>105</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>106</v>
-      </c>
-      <c r="H31" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
@@ -2223,21 +2228,21 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" t="s">
         <v>108</v>
-      </c>
-      <c r="G32" t="s">
-        <v>110</v>
-      </c>
-      <c r="H32" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -2247,24 +2252,24 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" t="s">
         <v>75</v>
-      </c>
-      <c r="G33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H33" t="s">
-        <v>114</v>
-      </c>
-      <c r="I33" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
@@ -2274,24 +2279,24 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" t="s">
         <v>111</v>
       </c>
-      <c r="G34" t="s">
-        <v>113</v>
-      </c>
-      <c r="H34" t="s">
-        <v>112</v>
-      </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="4">
         <v>1</v>
@@ -2301,21 +2306,21 @@
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" t="s">
         <v>94</v>
-      </c>
-      <c r="G35" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
@@ -2325,24 +2330,24 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" t="s">
+        <v>158</v>
+      </c>
+      <c r="H36" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" t="s">
         <v>159</v>
-      </c>
-      <c r="H36" t="s">
-        <v>158</v>
-      </c>
-      <c r="I36" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
@@ -2352,19 +2357,19 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F37" t="s">
+        <v>152</v>
+      </c>
+      <c r="G37" t="s">
         <v>153</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>154</v>
       </c>
-      <c r="H37" t="s">
-        <v>155</v>
-      </c>
       <c r="I37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -2377,35 +2382,35 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>